<commit_message>
dicionario de dados finalizado
</commit_message>
<xml_diff>
--- a/dicionario_de_dados/dicionario_de_dados.xlsx
+++ b/dicionario_de_dados/dicionario_de_dados.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Cliente\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Cliente\Documents\GitHub\projeto-modelagem-de-dados\dicionario_de_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2D096AA1-FC2E-46A9-BC2D-74FD80BDF10F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{45ECB23F-4ED3-45BE-B7FF-58D9D4F829E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DC90DC06-5CE6-474D-9341-360722F2D2F1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="127">
   <si>
     <t>tabelas</t>
   </si>
@@ -172,16 +172,256 @@
   </si>
   <si>
     <t>ças utilizadas)</t>
+  </si>
+  <si>
+    <t>tabela</t>
+  </si>
+  <si>
+    <t>atributos</t>
+  </si>
+  <si>
+    <t>restrições</t>
+  </si>
+  <si>
+    <t>id_cliente</t>
+  </si>
+  <si>
+    <t>modelo</t>
+  </si>
+  <si>
+    <t>marca</t>
+  </si>
+  <si>
+    <t>data_aquisição</t>
+  </si>
+  <si>
+    <t>ativo</t>
+  </si>
+  <si>
+    <t>FK</t>
+  </si>
+  <si>
+    <t>NOT NULL</t>
+  </si>
+  <si>
+    <t>tipo de dados</t>
+  </si>
+  <si>
+    <t>INT</t>
+  </si>
+  <si>
+    <t>VARCHAR(255)</t>
+  </si>
+  <si>
+    <t>DATE</t>
+  </si>
+  <si>
+    <t>BOOLEAN</t>
+  </si>
+  <si>
+    <t>modelo do carro</t>
+  </si>
+  <si>
+    <t>marca do carro</t>
+  </si>
+  <si>
+    <t>data da compra do carro</t>
+  </si>
+  <si>
+    <t>se o usuario ainda tem o carro ou não</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>nome</t>
+  </si>
+  <si>
+    <t>sobrenome</t>
+  </si>
+  <si>
+    <t>rua</t>
+  </si>
+  <si>
+    <t>bairro</t>
+  </si>
+  <si>
+    <t>numero_casa</t>
+  </si>
+  <si>
+    <t>NOT NULL, UNIQUE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> identificação do cliente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">identificação do cliente </t>
+  </si>
+  <si>
+    <t>primeiro nome do cliente</t>
+  </si>
+  <si>
+    <t>sobrenome do cliente</t>
+  </si>
+  <si>
+    <t>nome da rua onde o cliente mora</t>
+  </si>
+  <si>
+    <t>nome do bairro onde o cliente mora</t>
+  </si>
+  <si>
+    <t>numero da casa do cliente</t>
+  </si>
+  <si>
+    <t>id_departamento</t>
+  </si>
+  <si>
+    <t>identificação do funcionario</t>
+  </si>
+  <si>
+    <t>identificação do departamento</t>
+  </si>
+  <si>
+    <t>primeiro nome do funcionario</t>
+  </si>
+  <si>
+    <t>sobrenome do funcionario</t>
+  </si>
+  <si>
+    <t>nome da rua onde o funcionario mora</t>
+  </si>
+  <si>
+    <t>nome do bairro onde o funcionario mora</t>
+  </si>
+  <si>
+    <t>numero da casa do funcionario</t>
+  </si>
+  <si>
+    <t>custo_unitario</t>
+  </si>
+  <si>
+    <t>quantidade</t>
+  </si>
+  <si>
+    <t>veiculo_designado</t>
+  </si>
+  <si>
+    <t>identificação da peça</t>
+  </si>
+  <si>
+    <t>nome da peça</t>
+  </si>
+  <si>
+    <t>custo unitario(unidade) de uma peça</t>
+  </si>
+  <si>
+    <t>quantidade em estoque de uma peça</t>
+  </si>
+  <si>
+    <t>modelo do veiculo designado</t>
+  </si>
+  <si>
+    <t>preço_total</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>PK, AUTO_INCREMENT</t>
+  </si>
+  <si>
+    <t>identificação de cada reparação</t>
+  </si>
+  <si>
+    <t>preço_total_peça</t>
+  </si>
+  <si>
+    <t>preço total das peças utilizadas</t>
+  </si>
+  <si>
+    <t>preço total da reparação feita</t>
+  </si>
+  <si>
+    <t>data da reparação</t>
+  </si>
+  <si>
+    <t>carga_horaria</t>
+  </si>
+  <si>
+    <t>identificação de cada departamento</t>
+  </si>
+  <si>
+    <t>nome do departamento</t>
+  </si>
+  <si>
+    <t>carga horaria do departamento</t>
+  </si>
+  <si>
+    <t>telefone_residencial</t>
+  </si>
+  <si>
+    <t>telefone_profissional</t>
+  </si>
+  <si>
+    <t>telefone_pessoal</t>
+  </si>
+  <si>
+    <t>identificação de cada telefone</t>
+  </si>
+  <si>
+    <t>telefone da casa</t>
+  </si>
+  <si>
+    <t>telefone do trabalho</t>
+  </si>
+  <si>
+    <t>telefone pessoal(privado)</t>
+  </si>
+  <si>
+    <t>id_funcionario</t>
+  </si>
+  <si>
+    <t>id_reparação</t>
+  </si>
+  <si>
+    <t>id_peça</t>
+  </si>
+  <si>
+    <t>id_veiculo</t>
+  </si>
+  <si>
+    <t>identificação da reparação</t>
+  </si>
+  <si>
+    <t>identificação do veiculo</t>
+  </si>
+  <si>
+    <t>peças_utilizadas</t>
+  </si>
+  <si>
+    <t>tempo_gasto</t>
+  </si>
+  <si>
+    <t>peças utilizadas na reparação do veiculo</t>
+  </si>
+  <si>
+    <t>tempo total gasto na reparação</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -237,6 +477,160 @@
     <tableColumn id="2" xr3:uid="{533BF6AE-71B3-4E76-AB7E-214ABEDAE35D}" name="relacionamentos"/>
     <tableColumn id="3" xr3:uid="{383949E6-D4AE-4536-A55C-6E1385A7D5BA}" name="nome dos relacionamentos"/>
     <tableColumn id="4" xr3:uid="{515A53F2-D6D1-40DB-850E-A9A211743DBF}" name="descrição"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{C82CA65D-3D62-4726-831A-995D4EADDA88}" name="Tabela245678911" displayName="Tabela245678911" ref="A98:E101" totalsRowShown="0">
+  <autoFilter ref="A98:E101" xr:uid="{0F9E5768-B76E-41A7-8838-9FB043D9105E}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{ACB1D067-CDFE-494C-A898-32BAF258FB6E}" name="tabela"/>
+    <tableColumn id="2" xr3:uid="{17321485-2ABA-4172-B38D-19035AEAABB7}" name="atributos"/>
+    <tableColumn id="3" xr3:uid="{027B33AC-8F56-4190-A289-D7D25BEF90DD}" name="tipo de dados"/>
+    <tableColumn id="4" xr3:uid="{1FB5C5D4-58B6-4462-9C59-3D50C422D3CF}" name="restrições"/>
+    <tableColumn id="5" xr3:uid="{8736D108-E21C-47C2-9F6B-6BDF2EC75D9A}" name="descrição"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{9B1DBB9E-EC16-4BB7-8756-172EE09CC857}" name="Tabela24567891112" displayName="Tabela24567891112" ref="A104:E106" totalsRowShown="0">
+  <autoFilter ref="A104:E106" xr:uid="{BB703123-0F57-49A5-9E9D-AFB8FFDE4769}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{55F538C1-7897-43BE-83D0-398F242CCFF9}" name="tabela"/>
+    <tableColumn id="2" xr3:uid="{4102C002-9282-4FC3-936C-9D8E1AE700F2}" name="atributos"/>
+    <tableColumn id="3" xr3:uid="{8062FCFF-F330-4E2A-A392-72904694D1AE}" name="tipo de dados"/>
+    <tableColumn id="4" xr3:uid="{67DBFBCA-840E-43B2-A5D8-6DEBC182C060}" name="restrições"/>
+    <tableColumn id="5" xr3:uid="{433D2430-7B12-40DE-A283-4994FEE65F28}" name="descrição"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{64DD0B4A-DD31-4346-8ECD-4528902AB1D3}" name="Tabela2456789111213" displayName="Tabela2456789111213" ref="A109:E113" totalsRowShown="0">
+  <autoFilter ref="A109:E113" xr:uid="{4BD55DD5-108A-461C-A90A-66E744B3CC7E}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{09B541A8-6857-4153-8A36-AEF473973C7A}" name="tabela"/>
+    <tableColumn id="2" xr3:uid="{75B297D1-5603-4263-94C6-DD7B3F04817A}" name="atributos"/>
+    <tableColumn id="3" xr3:uid="{35E6126F-4160-4B7B-827F-68DDB24D5F28}" name="tipo de dados"/>
+    <tableColumn id="4" xr3:uid="{99C9F928-D6B1-408A-B651-DC98A175E927}" name="restrições"/>
+    <tableColumn id="5" xr3:uid="{41912C41-427C-4B0F-A67F-47DDCFB259F6}" name="descrição"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8ECD9B5D-D1DB-4C73-9FE8-E57F51DDCABB}" name="Tabela2" displayName="Tabela2" ref="A36:E41" totalsRowShown="0">
+  <autoFilter ref="A36:E41" xr:uid="{69F7608B-6DD3-48B4-8FB6-E23C98D3F205}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{B6CDB6A3-562A-49D5-A157-08E7873E3057}" name="tabela"/>
+    <tableColumn id="2" xr3:uid="{9612684E-8ADF-440B-B13F-C507442B7BB0}" name="atributos"/>
+    <tableColumn id="3" xr3:uid="{932E52DD-7428-4FB8-A45F-A15507CD8228}" name="tipo de dados"/>
+    <tableColumn id="4" xr3:uid="{CA87667C-E546-4CB9-AF65-32B2600EAAB6}" name="restrições"/>
+    <tableColumn id="5" xr3:uid="{911A3A36-6EA6-4A72-955F-181B96D6ED0F}" name="descrição"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{717404F2-FD36-4FAB-9D41-39F1423598E8}" name="Tabela24" displayName="Tabela24" ref="A44:E50" totalsRowShown="0">
+  <autoFilter ref="A44:E50" xr:uid="{5F4B1AE2-13A3-4659-9202-B9BDF15AEECE}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{5DE8470C-D6D1-4E67-A0A1-7F739C31E1C5}" name="tabela"/>
+    <tableColumn id="2" xr3:uid="{9E98B85E-589F-4893-B46C-74C1681564AB}" name="atributos"/>
+    <tableColumn id="3" xr3:uid="{DA97FD81-7A8B-44C7-A394-CC101F04F01A}" name="tipo de dados"/>
+    <tableColumn id="4" xr3:uid="{B143055F-FB59-491F-8084-A476B3697903}" name="restrições"/>
+    <tableColumn id="5" xr3:uid="{C772B83F-77C9-492E-9BAE-76B8D1F315C9}" name="descrição"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2556A190-A674-432E-A9B0-884FC06550C6}" name="Tabela245" displayName="Tabela245" ref="A53:E60" totalsRowShown="0">
+  <autoFilter ref="A53:E60" xr:uid="{F93B473B-C710-40E8-8159-1C6451D7A781}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{B82EAC89-E51B-4975-BF9E-05399C262959}" name="tabela"/>
+    <tableColumn id="2" xr3:uid="{3B38449E-9A24-4F23-A187-6AC7096E7578}" name="atributos"/>
+    <tableColumn id="3" xr3:uid="{52520414-5790-4B46-B029-2F04F7D0C38B}" name="tipo de dados"/>
+    <tableColumn id="4" xr3:uid="{D93388DC-D694-4937-9521-0D1EDE5E1EE2}" name="restrições"/>
+    <tableColumn id="5" xr3:uid="{321BA160-F9D6-42D5-9C0F-4C12B581B6D6}" name="descrição"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{916A28DD-6BE9-466B-9910-451CDE0A4D85}" name="Tabela2456" displayName="Tabela2456" ref="A63:E68" totalsRowShown="0">
+  <autoFilter ref="A63:E68" xr:uid="{C1E068CD-6B6B-420B-9E94-8C5A9AD20F4D}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{8DCBC6C2-B24F-481D-AF58-EB8F33796302}" name="tabela"/>
+    <tableColumn id="2" xr3:uid="{FAAA585B-CB3E-4171-9807-30596EAC0E49}" name="atributos"/>
+    <tableColumn id="3" xr3:uid="{A25FF08C-1557-411F-8C28-EB7A32CE52A5}" name="tipo de dados"/>
+    <tableColumn id="4" xr3:uid="{D412C4FE-2B45-4AE6-AC29-D243FF1FCF9F}" name="restrições"/>
+    <tableColumn id="5" xr3:uid="{438A3780-5B7C-4998-BBBC-C875E0638416}" name="descrição"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{CCF23B25-B2C8-4506-AD27-5DF12599BD1F}" name="Tabela24567" displayName="Tabela24567" ref="A71:E75" totalsRowShown="0">
+  <autoFilter ref="A71:E75" xr:uid="{49380DB2-D1B1-4886-A6C4-D5990FFAC44F}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{3A315230-1D5C-4F38-8D12-0A3759916029}" name="tabela"/>
+    <tableColumn id="2" xr3:uid="{215287C6-05C3-49E1-9139-CB9BB24D88B2}" name="atributos"/>
+    <tableColumn id="3" xr3:uid="{7D41BA71-8610-42CE-8D73-29055986C124}" name="tipo de dados"/>
+    <tableColumn id="4" xr3:uid="{3522836B-84FA-4156-97F5-644EE60F52F0}" name="restrições"/>
+    <tableColumn id="5" xr3:uid="{7A4F4E9C-947D-4D1F-BE07-FC625E803859}" name="descrição"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{FB95562A-6708-4C04-B0B4-6362F56A11E4}" name="Tabela245678" displayName="Tabela245678" ref="A78:E81" totalsRowShown="0">
+  <autoFilter ref="A78:E81" xr:uid="{4044E2E0-4558-4485-83EF-1E0D08285968}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{B11FDA2F-9086-4DE3-ABB2-DE31C0DD3380}" name="tabela"/>
+    <tableColumn id="2" xr3:uid="{634A9B8E-1611-4B35-A9CE-8781B4AA094E}" name="atributos"/>
+    <tableColumn id="3" xr3:uid="{102E0BB4-2ECF-4442-8DE6-B0B80E9CCF9E}" name="tipo de dados"/>
+    <tableColumn id="4" xr3:uid="{CFD7F93A-8E5D-4EF1-8275-4D7F9FB4E22F}" name="restrições"/>
+    <tableColumn id="5" xr3:uid="{B7FD68A4-AB8A-4587-AAC1-5A4B02983592}" name="descrição"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{2EAD4781-4502-4741-A96C-005D43F77B9C}" name="Tabela2456789" displayName="Tabela2456789" ref="A84:E88" totalsRowShown="0">
+  <autoFilter ref="A84:E88" xr:uid="{E4A23AAC-405A-4DED-9C3A-1495AD5DE75B}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{CB024A08-A906-40B7-A95F-CBF18D54067B}" name="tabela"/>
+    <tableColumn id="2" xr3:uid="{F92CCF0F-7472-4549-A737-0971809BBF3F}" name="atributos"/>
+    <tableColumn id="3" xr3:uid="{40913578-8425-42F2-85E9-277B3F1E574B}" name="tipo de dados"/>
+    <tableColumn id="4" xr3:uid="{0BACDAF4-B056-4912-8FFC-20DD6009C48B}" name="restrições"/>
+    <tableColumn id="5" xr3:uid="{1389C299-1D35-4BDA-871D-D007E49B4EE4}" name="descrição"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{868E7988-974F-42CC-B9FB-985B2AE38281}" name="Tabela245678910" displayName="Tabela245678910" ref="A91:E95" totalsRowShown="0">
+  <autoFilter ref="A91:E95" xr:uid="{E82CF52F-8D63-4A68-901A-CA462D2B2C0C}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{DBE8D966-24BC-4A85-B086-6E4C8A81A435}" name="tabela"/>
+    <tableColumn id="2" xr3:uid="{CFFC0C9F-04AE-4E89-A4FF-D5EB2FC5BD4D}" name="atributos"/>
+    <tableColumn id="3" xr3:uid="{2DC7F06F-6FFC-4ACA-A514-DC0C6E326228}" name="tipo de dados"/>
+    <tableColumn id="4" xr3:uid="{A4CBB1BA-4DA2-480C-80CE-A46001C887DD}" name="restrições"/>
+    <tableColumn id="5" xr3:uid="{5600036A-E085-4ADC-96B2-6602D21E64D1}" name="descrição"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -539,10 +933,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2932E057-6635-4611-B7BA-65D04C6C5CCB}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:E113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="D116" sqref="D116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,6 +945,7 @@
     <col min="2" max="2" width="31.140625" customWidth="1"/>
     <col min="3" max="3" width="27.5703125" customWidth="1"/>
     <col min="4" max="4" width="39" customWidth="1"/>
+    <col min="5" max="5" width="38.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -851,10 +1246,900 @@
         <v>48</v>
       </c>
     </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" t="s">
+        <v>51</v>
+      </c>
+      <c r="E36" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" t="s">
+        <v>60</v>
+      </c>
+      <c r="D37" t="s">
+        <v>57</v>
+      </c>
+      <c r="E37" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>53</v>
+      </c>
+      <c r="C38" t="s">
+        <v>61</v>
+      </c>
+      <c r="D38" t="s">
+        <v>58</v>
+      </c>
+      <c r="E38" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>54</v>
+      </c>
+      <c r="C39" t="s">
+        <v>61</v>
+      </c>
+      <c r="D39" t="s">
+        <v>58</v>
+      </c>
+      <c r="E39" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" t="s">
+        <v>62</v>
+      </c>
+      <c r="D40" t="s">
+        <v>58</v>
+      </c>
+      <c r="E40" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>56</v>
+      </c>
+      <c r="C41" t="s">
+        <v>63</v>
+      </c>
+      <c r="D41" t="s">
+        <v>58</v>
+      </c>
+      <c r="E41" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44" t="s">
+        <v>50</v>
+      </c>
+      <c r="C44" t="s">
+        <v>59</v>
+      </c>
+      <c r="D44" t="s">
+        <v>51</v>
+      </c>
+      <c r="E44" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" t="s">
+        <v>68</v>
+      </c>
+      <c r="C45" t="s">
+        <v>60</v>
+      </c>
+      <c r="D45" t="s">
+        <v>100</v>
+      </c>
+      <c r="E45" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>69</v>
+      </c>
+      <c r="C46" t="s">
+        <v>61</v>
+      </c>
+      <c r="D46" t="s">
+        <v>58</v>
+      </c>
+      <c r="E46" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>70</v>
+      </c>
+      <c r="C47" t="s">
+        <v>61</v>
+      </c>
+      <c r="D47" t="s">
+        <v>58</v>
+      </c>
+      <c r="E47" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>71</v>
+      </c>
+      <c r="C48" t="s">
+        <v>61</v>
+      </c>
+      <c r="D48" t="s">
+        <v>58</v>
+      </c>
+      <c r="E48" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>72</v>
+      </c>
+      <c r="C49" t="s">
+        <v>61</v>
+      </c>
+      <c r="D49" t="s">
+        <v>58</v>
+      </c>
+      <c r="E49" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>73</v>
+      </c>
+      <c r="C50" t="s">
+        <v>60</v>
+      </c>
+      <c r="D50" t="s">
+        <v>74</v>
+      </c>
+      <c r="E50" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>49</v>
+      </c>
+      <c r="B53" t="s">
+        <v>50</v>
+      </c>
+      <c r="C53" t="s">
+        <v>59</v>
+      </c>
+      <c r="D53" t="s">
+        <v>51</v>
+      </c>
+      <c r="E53" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>14</v>
+      </c>
+      <c r="B54" t="s">
+        <v>68</v>
+      </c>
+      <c r="C54" t="s">
+        <v>60</v>
+      </c>
+      <c r="D54" t="s">
+        <v>100</v>
+      </c>
+      <c r="E54" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>82</v>
+      </c>
+      <c r="C55" t="s">
+        <v>60</v>
+      </c>
+      <c r="D55" t="s">
+        <v>57</v>
+      </c>
+      <c r="E55" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>69</v>
+      </c>
+      <c r="C56" t="s">
+        <v>61</v>
+      </c>
+      <c r="D56" t="s">
+        <v>58</v>
+      </c>
+      <c r="E56" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>70</v>
+      </c>
+      <c r="C57" t="s">
+        <v>61</v>
+      </c>
+      <c r="D57" t="s">
+        <v>58</v>
+      </c>
+      <c r="E57" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>71</v>
+      </c>
+      <c r="C58" t="s">
+        <v>61</v>
+      </c>
+      <c r="D58" t="s">
+        <v>58</v>
+      </c>
+      <c r="E58" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>72</v>
+      </c>
+      <c r="C59" t="s">
+        <v>61</v>
+      </c>
+      <c r="D59" t="s">
+        <v>58</v>
+      </c>
+      <c r="E59" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>73</v>
+      </c>
+      <c r="C60" t="s">
+        <v>60</v>
+      </c>
+      <c r="D60" t="s">
+        <v>74</v>
+      </c>
+      <c r="E60" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>49</v>
+      </c>
+      <c r="B63" t="s">
+        <v>50</v>
+      </c>
+      <c r="C63" t="s">
+        <v>59</v>
+      </c>
+      <c r="D63" t="s">
+        <v>51</v>
+      </c>
+      <c r="E63" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>24</v>
+      </c>
+      <c r="B64" t="s">
+        <v>68</v>
+      </c>
+      <c r="C64" t="s">
+        <v>60</v>
+      </c>
+      <c r="D64" t="s">
+        <v>100</v>
+      </c>
+      <c r="E64" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>90</v>
+      </c>
+      <c r="C65" t="s">
+        <v>60</v>
+      </c>
+      <c r="D65" t="s">
+        <v>58</v>
+      </c>
+      <c r="E65" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>69</v>
+      </c>
+      <c r="C66" t="s">
+        <v>61</v>
+      </c>
+      <c r="D66" t="s">
+        <v>58</v>
+      </c>
+      <c r="E66" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>91</v>
+      </c>
+      <c r="C67" t="s">
+        <v>60</v>
+      </c>
+      <c r="D67" t="s">
+        <v>58</v>
+      </c>
+      <c r="E67" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>92</v>
+      </c>
+      <c r="C68" t="s">
+        <v>61</v>
+      </c>
+      <c r="D68" t="s">
+        <v>74</v>
+      </c>
+      <c r="E68" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>49</v>
+      </c>
+      <c r="B71" t="s">
+        <v>50</v>
+      </c>
+      <c r="C71" t="s">
+        <v>59</v>
+      </c>
+      <c r="D71" t="s">
+        <v>51</v>
+      </c>
+      <c r="E71" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>29</v>
+      </c>
+      <c r="B72" t="s">
+        <v>68</v>
+      </c>
+      <c r="C72" t="s">
+        <v>60</v>
+      </c>
+      <c r="D72" t="s">
+        <v>100</v>
+      </c>
+      <c r="E72" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>102</v>
+      </c>
+      <c r="C73" t="s">
+        <v>61</v>
+      </c>
+      <c r="D73" t="s">
+        <v>58</v>
+      </c>
+      <c r="E73" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>98</v>
+      </c>
+      <c r="C74" t="s">
+        <v>61</v>
+      </c>
+      <c r="D74" t="s">
+        <v>58</v>
+      </c>
+      <c r="E74" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>99</v>
+      </c>
+      <c r="C75" t="s">
+        <v>62</v>
+      </c>
+      <c r="D75" t="s">
+        <v>58</v>
+      </c>
+      <c r="E75" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>49</v>
+      </c>
+      <c r="B78" t="s">
+        <v>50</v>
+      </c>
+      <c r="C78" t="s">
+        <v>59</v>
+      </c>
+      <c r="D78" t="s">
+        <v>51</v>
+      </c>
+      <c r="E78" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>15</v>
+      </c>
+      <c r="B79" t="s">
+        <v>68</v>
+      </c>
+      <c r="C79" t="s">
+        <v>60</v>
+      </c>
+      <c r="D79" t="s">
+        <v>100</v>
+      </c>
+      <c r="E79" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>69</v>
+      </c>
+      <c r="C80" t="s">
+        <v>61</v>
+      </c>
+      <c r="D80" t="s">
+        <v>74</v>
+      </c>
+      <c r="E80" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>106</v>
+      </c>
+      <c r="C81" t="s">
+        <v>61</v>
+      </c>
+      <c r="D81" t="s">
+        <v>58</v>
+      </c>
+      <c r="E81" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>49</v>
+      </c>
+      <c r="B84" t="s">
+        <v>50</v>
+      </c>
+      <c r="C84" t="s">
+        <v>59</v>
+      </c>
+      <c r="D84" t="s">
+        <v>51</v>
+      </c>
+      <c r="E84" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>9</v>
+      </c>
+      <c r="B85" t="s">
+        <v>52</v>
+      </c>
+      <c r="C85" t="s">
+        <v>60</v>
+      </c>
+      <c r="D85" t="s">
+        <v>57</v>
+      </c>
+      <c r="E85" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>110</v>
+      </c>
+      <c r="C86" t="s">
+        <v>61</v>
+      </c>
+      <c r="D86" t="s">
+        <v>74</v>
+      </c>
+      <c r="E86" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>111</v>
+      </c>
+      <c r="C87" t="s">
+        <v>61</v>
+      </c>
+      <c r="D87" t="s">
+        <v>74</v>
+      </c>
+      <c r="E87" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>112</v>
+      </c>
+      <c r="C88" t="s">
+        <v>61</v>
+      </c>
+      <c r="D88" t="s">
+        <v>74</v>
+      </c>
+      <c r="E88" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>49</v>
+      </c>
+      <c r="B91" t="s">
+        <v>50</v>
+      </c>
+      <c r="C91" t="s">
+        <v>59</v>
+      </c>
+      <c r="D91" t="s">
+        <v>51</v>
+      </c>
+      <c r="E91" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>17</v>
+      </c>
+      <c r="B92" t="s">
+        <v>117</v>
+      </c>
+      <c r="C92" t="s">
+        <v>60</v>
+      </c>
+      <c r="D92" t="s">
+        <v>57</v>
+      </c>
+      <c r="E92" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>110</v>
+      </c>
+      <c r="C93" t="s">
+        <v>61</v>
+      </c>
+      <c r="D93" t="s">
+        <v>74</v>
+      </c>
+      <c r="E93" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>111</v>
+      </c>
+      <c r="C94" t="s">
+        <v>61</v>
+      </c>
+      <c r="D94" t="s">
+        <v>74</v>
+      </c>
+      <c r="E94" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>112</v>
+      </c>
+      <c r="C95" t="s">
+        <v>61</v>
+      </c>
+      <c r="D95" t="s">
+        <v>74</v>
+      </c>
+      <c r="E95" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>49</v>
+      </c>
+      <c r="B98" t="s">
+        <v>50</v>
+      </c>
+      <c r="C98" t="s">
+        <v>59</v>
+      </c>
+      <c r="D98" t="s">
+        <v>51</v>
+      </c>
+      <c r="E98" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>25</v>
+      </c>
+      <c r="B99" t="s">
+        <v>118</v>
+      </c>
+      <c r="C99" t="s">
+        <v>60</v>
+      </c>
+      <c r="D99" t="s">
+        <v>57</v>
+      </c>
+      <c r="E99" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>119</v>
+      </c>
+      <c r="C100" t="s">
+        <v>60</v>
+      </c>
+      <c r="D100" t="s">
+        <v>57</v>
+      </c>
+      <c r="E100" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>120</v>
+      </c>
+      <c r="C101" t="s">
+        <v>60</v>
+      </c>
+      <c r="D101" t="s">
+        <v>57</v>
+      </c>
+      <c r="E101" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>49</v>
+      </c>
+      <c r="B104" t="s">
+        <v>50</v>
+      </c>
+      <c r="C104" t="s">
+        <v>59</v>
+      </c>
+      <c r="D104" t="s">
+        <v>51</v>
+      </c>
+      <c r="E104" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>5</v>
+      </c>
+      <c r="B105" t="s">
+        <v>118</v>
+      </c>
+      <c r="C105" t="s">
+        <v>60</v>
+      </c>
+      <c r="D105" t="s">
+        <v>57</v>
+      </c>
+      <c r="E105" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
+        <v>120</v>
+      </c>
+      <c r="C106" t="s">
+        <v>60</v>
+      </c>
+      <c r="D106" t="s">
+        <v>57</v>
+      </c>
+      <c r="E106" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>49</v>
+      </c>
+      <c r="B109" t="s">
+        <v>50</v>
+      </c>
+      <c r="C109" t="s">
+        <v>59</v>
+      </c>
+      <c r="D109" t="s">
+        <v>51</v>
+      </c>
+      <c r="E109" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>30</v>
+      </c>
+      <c r="B110" t="s">
+        <v>118</v>
+      </c>
+      <c r="C110" t="s">
+        <v>60</v>
+      </c>
+      <c r="D110" t="s">
+        <v>57</v>
+      </c>
+      <c r="E110" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B111" t="s">
+        <v>117</v>
+      </c>
+      <c r="C111" t="s">
+        <v>60</v>
+      </c>
+      <c r="D111" t="s">
+        <v>57</v>
+      </c>
+      <c r="E111" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B112" t="s">
+        <v>123</v>
+      </c>
+      <c r="C112" t="s">
+        <v>60</v>
+      </c>
+      <c r="D112" t="s">
+        <v>58</v>
+      </c>
+      <c r="E112" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="113" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
+        <v>124</v>
+      </c>
+      <c r="C113" t="s">
+        <v>61</v>
+      </c>
+      <c r="D113" t="s">
+        <v>58</v>
+      </c>
+      <c r="E113" t="s">
+        <v>126</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <tableParts count="1">
+  <tableParts count="12">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
+    <tablePart r:id="rId12"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
alterei alguns atributos(dicionario de dados)
</commit_message>
<xml_diff>
--- a/dicionario_de_dados/dicionario_de_dados.xlsx
+++ b/dicionario_de_dados/dicionario_de_dados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Cliente\Documents\GitHub\projeto-modelagem-de-dados\dicionario_de_dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{45ECB23F-4ED3-45BE-B7FF-58D9D4F829E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C2C187A6-7BA9-45B5-AD2C-923D44EFB09E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DC90DC06-5CE6-474D-9341-360722F2D2F1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="129">
   <si>
     <t>tabelas</t>
   </si>
@@ -406,6 +406,12 @@
   </si>
   <si>
     <t>tempo total gasto na reparação</t>
+  </si>
+  <si>
+    <t>UNIQUE</t>
+  </si>
+  <si>
+    <t>PK</t>
   </si>
 </sst>
 </file>
@@ -483,8 +489,8 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{C82CA65D-3D62-4726-831A-995D4EADDA88}" name="Tabela245678911" displayName="Tabela245678911" ref="A98:E101" totalsRowShown="0">
-  <autoFilter ref="A98:E101" xr:uid="{0F9E5768-B76E-41A7-8838-9FB043D9105E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{C82CA65D-3D62-4726-831A-995D4EADDA88}" name="Tabela245678911" displayName="Tabela245678911" ref="A99:E102" totalsRowShown="0">
+  <autoFilter ref="A99:E102" xr:uid="{0F9E5768-B76E-41A7-8838-9FB043D9105E}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{ACB1D067-CDFE-494C-A898-32BAF258FB6E}" name="tabela"/>
     <tableColumn id="2" xr3:uid="{17321485-2ABA-4172-B38D-19035AEAABB7}" name="atributos"/>
@@ -497,8 +503,8 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{9B1DBB9E-EC16-4BB7-8756-172EE09CC857}" name="Tabela24567891112" displayName="Tabela24567891112" ref="A104:E106" totalsRowShown="0">
-  <autoFilter ref="A104:E106" xr:uid="{BB703123-0F57-49A5-9E9D-AFB8FFDE4769}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{9B1DBB9E-EC16-4BB7-8756-172EE09CC857}" name="Tabela24567891112" displayName="Tabela24567891112" ref="A105:E107" totalsRowShown="0">
+  <autoFilter ref="A105:E107" xr:uid="{BB703123-0F57-49A5-9E9D-AFB8FFDE4769}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{55F538C1-7897-43BE-83D0-398F242CCFF9}" name="tabela"/>
     <tableColumn id="2" xr3:uid="{4102C002-9282-4FC3-936C-9D8E1AE700F2}" name="atributos"/>
@@ -511,8 +517,8 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{64DD0B4A-DD31-4346-8ECD-4528902AB1D3}" name="Tabela2456789111213" displayName="Tabela2456789111213" ref="A109:E113" totalsRowShown="0">
-  <autoFilter ref="A109:E113" xr:uid="{4BD55DD5-108A-461C-A90A-66E744B3CC7E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{64DD0B4A-DD31-4346-8ECD-4528902AB1D3}" name="Tabela2456789111213" displayName="Tabela2456789111213" ref="A110:E114" totalsRowShown="0">
+  <autoFilter ref="A110:E114" xr:uid="{4BD55DD5-108A-461C-A90A-66E744B3CC7E}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{09B541A8-6857-4153-8A36-AEF473973C7A}" name="tabela"/>
     <tableColumn id="2" xr3:uid="{75B297D1-5603-4263-94C6-DD7B3F04817A}" name="atributos"/>
@@ -525,8 +531,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8ECD9B5D-D1DB-4C73-9FE8-E57F51DDCABB}" name="Tabela2" displayName="Tabela2" ref="A36:E41" totalsRowShown="0">
-  <autoFilter ref="A36:E41" xr:uid="{69F7608B-6DD3-48B4-8FB6-E23C98D3F205}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{8ECD9B5D-D1DB-4C73-9FE8-E57F51DDCABB}" name="Tabela2" displayName="Tabela2" ref="A36:E42" totalsRowShown="0">
+  <autoFilter ref="A36:E42" xr:uid="{69F7608B-6DD3-48B4-8FB6-E23C98D3F205}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{B6CDB6A3-562A-49D5-A157-08E7873E3057}" name="tabela"/>
     <tableColumn id="2" xr3:uid="{9612684E-8ADF-440B-B13F-C507442B7BB0}" name="atributos"/>
@@ -539,8 +545,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{717404F2-FD36-4FAB-9D41-39F1423598E8}" name="Tabela24" displayName="Tabela24" ref="A44:E50" totalsRowShown="0">
-  <autoFilter ref="A44:E50" xr:uid="{5F4B1AE2-13A3-4659-9202-B9BDF15AEECE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{717404F2-FD36-4FAB-9D41-39F1423598E8}" name="Tabela24" displayName="Tabela24" ref="A45:E51" totalsRowShown="0">
+  <autoFilter ref="A45:E51" xr:uid="{5F4B1AE2-13A3-4659-9202-B9BDF15AEECE}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{5DE8470C-D6D1-4E67-A0A1-7F739C31E1C5}" name="tabela"/>
     <tableColumn id="2" xr3:uid="{9E98B85E-589F-4893-B46C-74C1681564AB}" name="atributos"/>
@@ -553,8 +559,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2556A190-A674-432E-A9B0-884FC06550C6}" name="Tabela245" displayName="Tabela245" ref="A53:E60" totalsRowShown="0">
-  <autoFilter ref="A53:E60" xr:uid="{F93B473B-C710-40E8-8159-1C6451D7A781}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{2556A190-A674-432E-A9B0-884FC06550C6}" name="Tabela245" displayName="Tabela245" ref="A54:E61" totalsRowShown="0">
+  <autoFilter ref="A54:E61" xr:uid="{F93B473B-C710-40E8-8159-1C6451D7A781}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{B82EAC89-E51B-4975-BF9E-05399C262959}" name="tabela"/>
     <tableColumn id="2" xr3:uid="{3B38449E-9A24-4F23-A187-6AC7096E7578}" name="atributos"/>
@@ -567,8 +573,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{916A28DD-6BE9-466B-9910-451CDE0A4D85}" name="Tabela2456" displayName="Tabela2456" ref="A63:E68" totalsRowShown="0">
-  <autoFilter ref="A63:E68" xr:uid="{C1E068CD-6B6B-420B-9E94-8C5A9AD20F4D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{916A28DD-6BE9-466B-9910-451CDE0A4D85}" name="Tabela2456" displayName="Tabela2456" ref="A64:E69" totalsRowShown="0">
+  <autoFilter ref="A64:E69" xr:uid="{C1E068CD-6B6B-420B-9E94-8C5A9AD20F4D}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{8DCBC6C2-B24F-481D-AF58-EB8F33796302}" name="tabela"/>
     <tableColumn id="2" xr3:uid="{FAAA585B-CB3E-4171-9807-30596EAC0E49}" name="atributos"/>
@@ -581,8 +587,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{CCF23B25-B2C8-4506-AD27-5DF12599BD1F}" name="Tabela24567" displayName="Tabela24567" ref="A71:E75" totalsRowShown="0">
-  <autoFilter ref="A71:E75" xr:uid="{49380DB2-D1B1-4886-A6C4-D5990FFAC44F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{CCF23B25-B2C8-4506-AD27-5DF12599BD1F}" name="Tabela24567" displayName="Tabela24567" ref="A72:E76" totalsRowShown="0">
+  <autoFilter ref="A72:E76" xr:uid="{49380DB2-D1B1-4886-A6C4-D5990FFAC44F}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{3A315230-1D5C-4F38-8D12-0A3759916029}" name="tabela"/>
     <tableColumn id="2" xr3:uid="{215287C6-05C3-49E1-9139-CB9BB24D88B2}" name="atributos"/>
@@ -595,8 +601,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{FB95562A-6708-4C04-B0B4-6362F56A11E4}" name="Tabela245678" displayName="Tabela245678" ref="A78:E81" totalsRowShown="0">
-  <autoFilter ref="A78:E81" xr:uid="{4044E2E0-4558-4485-83EF-1E0D08285968}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{FB95562A-6708-4C04-B0B4-6362F56A11E4}" name="Tabela245678" displayName="Tabela245678" ref="A79:E82" totalsRowShown="0">
+  <autoFilter ref="A79:E82" xr:uid="{4044E2E0-4558-4485-83EF-1E0D08285968}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{B11FDA2F-9086-4DE3-ABB2-DE31C0DD3380}" name="tabela"/>
     <tableColumn id="2" xr3:uid="{634A9B8E-1611-4B35-A9CE-8781B4AA094E}" name="atributos"/>
@@ -609,8 +615,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{2EAD4781-4502-4741-A96C-005D43F77B9C}" name="Tabela2456789" displayName="Tabela2456789" ref="A84:E88" totalsRowShown="0">
-  <autoFilter ref="A84:E88" xr:uid="{E4A23AAC-405A-4DED-9C3A-1495AD5DE75B}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{2EAD4781-4502-4741-A96C-005D43F77B9C}" name="Tabela2456789" displayName="Tabela2456789" ref="A85:E89" totalsRowShown="0">
+  <autoFilter ref="A85:E89" xr:uid="{E4A23AAC-405A-4DED-9C3A-1495AD5DE75B}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{CB024A08-A906-40B7-A95F-CBF18D54067B}" name="tabela"/>
     <tableColumn id="2" xr3:uid="{F92CCF0F-7472-4549-A737-0971809BBF3F}" name="atributos"/>
@@ -623,8 +629,8 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{868E7988-974F-42CC-B9FB-985B2AE38281}" name="Tabela245678910" displayName="Tabela245678910" ref="A91:E95" totalsRowShown="0">
-  <autoFilter ref="A91:E95" xr:uid="{E82CF52F-8D63-4A68-901A-CA462D2B2C0C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{868E7988-974F-42CC-B9FB-985B2AE38281}" name="Tabela245678910" displayName="Tabela245678910" ref="A92:E96" totalsRowShown="0">
+  <autoFilter ref="A92:E96" xr:uid="{E82CF52F-8D63-4A68-901A-CA462D2B2C0C}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{DBE8D966-24BC-4A85-B086-6E4C8A81A435}" name="tabela"/>
     <tableColumn id="2" xr3:uid="{CFFC0C9F-04AE-4E89-A4FF-D5EB2FC5BD4D}" name="atributos"/>
@@ -933,10 +939,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2932E057-6635-4611-B7BA-65D04C6C5CCB}">
-  <dimension ref="A1:E113"/>
+  <dimension ref="A1:E114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="D116" sqref="D116"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1268,35 +1274,35 @@
         <v>4</v>
       </c>
       <c r="B37" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="C37" t="s">
         <v>60</v>
       </c>
       <c r="D37" t="s">
-        <v>57</v>
+        <v>128</v>
       </c>
       <c r="E37" t="s">
-        <v>76</v>
+        <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E38" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C39" t="s">
         <v>61</v>
@@ -1305,88 +1311,88 @@
         <v>58</v>
       </c>
       <c r="E39" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C40" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D40" t="s">
         <v>58</v>
       </c>
       <c r="E40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D41" t="s">
         <v>58</v>
       </c>
       <c r="E41" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>56</v>
+      </c>
+      <c r="C42" t="s">
+        <v>63</v>
+      </c>
+      <c r="D42" t="s">
+        <v>58</v>
+      </c>
+      <c r="E42" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>49</v>
-      </c>
-      <c r="B44" t="s">
-        <v>50</v>
-      </c>
-      <c r="C44" t="s">
-        <v>59</v>
-      </c>
-      <c r="D44" t="s">
-        <v>51</v>
-      </c>
-      <c r="E44" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>49</v>
+      </c>
+      <c r="B45" t="s">
+        <v>50</v>
+      </c>
+      <c r="C45" t="s">
+        <v>59</v>
+      </c>
+      <c r="D45" t="s">
+        <v>51</v>
+      </c>
+      <c r="E45" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>6</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>68</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>60</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D46" t="s">
         <v>100</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E46" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>69</v>
-      </c>
-      <c r="C46" t="s">
-        <v>61</v>
-      </c>
-      <c r="D46" t="s">
-        <v>58</v>
-      </c>
-      <c r="E46" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C47" t="s">
         <v>61</v>
@@ -1395,12 +1401,12 @@
         <v>58</v>
       </c>
       <c r="E47" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C48" t="s">
         <v>61</v>
@@ -1409,12 +1415,12 @@
         <v>58</v>
       </c>
       <c r="E48" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C49" t="s">
         <v>61</v>
@@ -1423,88 +1429,88 @@
         <v>58</v>
       </c>
       <c r="E49" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
+        <v>72</v>
+      </c>
+      <c r="C50" t="s">
+        <v>61</v>
+      </c>
+      <c r="D50" t="s">
+        <v>58</v>
+      </c>
+      <c r="E50" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
         <v>73</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C51" t="s">
         <v>60</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D51" t="s">
         <v>74</v>
       </c>
-      <c r="E50" t="s">
+      <c r="E51" t="s">
         <v>81</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>49</v>
-      </c>
-      <c r="B53" t="s">
-        <v>50</v>
-      </c>
-      <c r="C53" t="s">
-        <v>59</v>
-      </c>
-      <c r="D53" t="s">
-        <v>51</v>
-      </c>
-      <c r="E53" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>49</v>
+      </c>
+      <c r="B54" t="s">
+        <v>50</v>
+      </c>
+      <c r="C54" t="s">
+        <v>59</v>
+      </c>
+      <c r="D54" t="s">
+        <v>51</v>
+      </c>
+      <c r="E54" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>14</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>68</v>
-      </c>
-      <c r="C54" t="s">
-        <v>60</v>
-      </c>
-      <c r="D54" t="s">
-        <v>100</v>
-      </c>
-      <c r="E54" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>82</v>
       </c>
       <c r="C55" t="s">
         <v>60</v>
       </c>
       <c r="D55" t="s">
-        <v>57</v>
+        <v>100</v>
       </c>
       <c r="E55" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>69</v>
+        <v>82</v>
       </c>
       <c r="C56" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D56" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E56" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C57" t="s">
         <v>61</v>
@@ -1513,12 +1519,12 @@
         <v>58</v>
       </c>
       <c r="E57" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C58" t="s">
         <v>61</v>
@@ -1527,12 +1533,12 @@
         <v>58</v>
       </c>
       <c r="E58" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C59" t="s">
         <v>61</v>
@@ -1541,164 +1547,164 @@
         <v>58</v>
       </c>
       <c r="E59" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
+        <v>72</v>
+      </c>
+      <c r="C60" t="s">
+        <v>61</v>
+      </c>
+      <c r="D60" t="s">
+        <v>58</v>
+      </c>
+      <c r="E60" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
         <v>73</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C61" t="s">
         <v>60</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D61" t="s">
         <v>74</v>
       </c>
-      <c r="E60" t="s">
+      <c r="E61" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>49</v>
-      </c>
-      <c r="B63" t="s">
-        <v>50</v>
-      </c>
-      <c r="C63" t="s">
-        <v>59</v>
-      </c>
-      <c r="D63" t="s">
-        <v>51</v>
-      </c>
-      <c r="E63" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>49</v>
+      </c>
+      <c r="B64" t="s">
+        <v>50</v>
+      </c>
+      <c r="C64" t="s">
+        <v>59</v>
+      </c>
+      <c r="D64" t="s">
+        <v>51</v>
+      </c>
+      <c r="E64" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>24</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" t="s">
         <v>68</v>
-      </c>
-      <c r="C64" t="s">
-        <v>60</v>
-      </c>
-      <c r="D64" t="s">
-        <v>100</v>
-      </c>
-      <c r="E64" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
-        <v>90</v>
       </c>
       <c r="C65" t="s">
         <v>60</v>
       </c>
       <c r="D65" t="s">
-        <v>58</v>
+        <v>100</v>
       </c>
       <c r="E65" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>69</v>
+        <v>90</v>
       </c>
       <c r="C66" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D66" t="s">
         <v>58</v>
       </c>
       <c r="E66" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="C67" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D67" t="s">
         <v>58</v>
       </c>
       <c r="E67" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
+        <v>91</v>
+      </c>
+      <c r="C68" t="s">
+        <v>60</v>
+      </c>
+      <c r="D68" t="s">
+        <v>58</v>
+      </c>
+      <c r="E68" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
         <v>92</v>
       </c>
-      <c r="C68" t="s">
-        <v>61</v>
-      </c>
-      <c r="D68" t="s">
+      <c r="C69" t="s">
+        <v>61</v>
+      </c>
+      <c r="D69" t="s">
         <v>74</v>
       </c>
-      <c r="E68" t="s">
+      <c r="E69" t="s">
         <v>97</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>49</v>
-      </c>
-      <c r="B71" t="s">
-        <v>50</v>
-      </c>
-      <c r="C71" t="s">
-        <v>59</v>
-      </c>
-      <c r="D71" t="s">
-        <v>51</v>
-      </c>
-      <c r="E71" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>49</v>
+      </c>
+      <c r="B72" t="s">
+        <v>50</v>
+      </c>
+      <c r="C72" t="s">
+        <v>59</v>
+      </c>
+      <c r="D72" t="s">
+        <v>51</v>
+      </c>
+      <c r="E72" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>29</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B73" t="s">
         <v>68</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C73" t="s">
         <v>60</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D73" t="s">
         <v>100</v>
       </c>
-      <c r="E72" t="s">
+      <c r="E73" t="s">
         <v>101</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
-        <v>102</v>
-      </c>
-      <c r="C73" t="s">
-        <v>61</v>
-      </c>
-      <c r="D73" t="s">
-        <v>58</v>
-      </c>
-      <c r="E73" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C74" t="s">
         <v>61</v>
@@ -1707,212 +1713,212 @@
         <v>58</v>
       </c>
       <c r="E74" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C75" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D75" t="s">
         <v>58</v>
       </c>
       <c r="E75" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>99</v>
+      </c>
+      <c r="C76" t="s">
+        <v>62</v>
+      </c>
+      <c r="D76" t="s">
+        <v>58</v>
+      </c>
+      <c r="E76" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>49</v>
-      </c>
-      <c r="B78" t="s">
-        <v>50</v>
-      </c>
-      <c r="C78" t="s">
-        <v>59</v>
-      </c>
-      <c r="D78" t="s">
-        <v>51</v>
-      </c>
-      <c r="E78" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>49</v>
+      </c>
+      <c r="B79" t="s">
+        <v>50</v>
+      </c>
+      <c r="C79" t="s">
+        <v>59</v>
+      </c>
+      <c r="D79" t="s">
+        <v>51</v>
+      </c>
+      <c r="E79" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>15</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B80" t="s">
         <v>68</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C80" t="s">
         <v>60</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D80" t="s">
         <v>100</v>
       </c>
-      <c r="E79" t="s">
+      <c r="E80" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B80" t="s">
-        <v>69</v>
-      </c>
-      <c r="C80" t="s">
-        <v>61</v>
-      </c>
-      <c r="D80" t="s">
-        <v>74</v>
-      </c>
-      <c r="E80" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
+        <v>69</v>
+      </c>
+      <c r="C81" t="s">
+        <v>61</v>
+      </c>
+      <c r="D81" t="s">
+        <v>74</v>
+      </c>
+      <c r="E81" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
         <v>106</v>
       </c>
-      <c r="C81" t="s">
-        <v>61</v>
-      </c>
-      <c r="D81" t="s">
+      <c r="C82" t="s">
+        <v>61</v>
+      </c>
+      <c r="D82" t="s">
         <v>58</v>
       </c>
-      <c r="E81" t="s">
+      <c r="E82" t="s">
         <v>109</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>49</v>
-      </c>
-      <c r="B84" t="s">
-        <v>50</v>
-      </c>
-      <c r="C84" t="s">
-        <v>59</v>
-      </c>
-      <c r="D84" t="s">
-        <v>51</v>
-      </c>
-      <c r="E84" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
+        <v>49</v>
+      </c>
+      <c r="B85" t="s">
+        <v>50</v>
+      </c>
+      <c r="C85" t="s">
+        <v>59</v>
+      </c>
+      <c r="D85" t="s">
+        <v>51</v>
+      </c>
+      <c r="E85" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
         <v>9</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B86" t="s">
         <v>52</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C86" t="s">
         <v>60</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D86" t="s">
         <v>57</v>
       </c>
-      <c r="E85" t="s">
+      <c r="E86" t="s">
         <v>113</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B86" t="s">
-        <v>110</v>
-      </c>
-      <c r="C86" t="s">
-        <v>61</v>
-      </c>
-      <c r="D86" t="s">
-        <v>74</v>
-      </c>
-      <c r="E86" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C87" t="s">
         <v>61</v>
       </c>
       <c r="D87" t="s">
-        <v>74</v>
+        <v>127</v>
       </c>
       <c r="E87" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
+        <v>111</v>
+      </c>
+      <c r="C88" t="s">
+        <v>61</v>
+      </c>
+      <c r="D88" t="s">
+        <v>127</v>
+      </c>
+      <c r="E88" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
         <v>112</v>
       </c>
-      <c r="C88" t="s">
-        <v>61</v>
-      </c>
-      <c r="D88" t="s">
+      <c r="C89" t="s">
+        <v>61</v>
+      </c>
+      <c r="D89" t="s">
         <v>74</v>
       </c>
-      <c r="E88" t="s">
+      <c r="E89" t="s">
         <v>116</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>49</v>
-      </c>
-      <c r="B91" t="s">
-        <v>50</v>
-      </c>
-      <c r="C91" t="s">
-        <v>59</v>
-      </c>
-      <c r="D91" t="s">
-        <v>51</v>
-      </c>
-      <c r="E91" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
+        <v>49</v>
+      </c>
+      <c r="B92" t="s">
+        <v>50</v>
+      </c>
+      <c r="C92" t="s">
+        <v>59</v>
+      </c>
+      <c r="D92" t="s">
+        <v>51</v>
+      </c>
+      <c r="E92" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>17</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B93" t="s">
         <v>117</v>
       </c>
-      <c r="C92" t="s">
+      <c r="C93" t="s">
         <v>60</v>
       </c>
-      <c r="D92" t="s">
+      <c r="D93" t="s">
         <v>57</v>
       </c>
-      <c r="E92" t="s">
+      <c r="E93" t="s">
         <v>113</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B93" t="s">
-        <v>110</v>
-      </c>
-      <c r="C93" t="s">
-        <v>61</v>
-      </c>
-      <c r="D93" t="s">
-        <v>74</v>
-      </c>
-      <c r="E93" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C94" t="s">
         <v>61</v>
@@ -1921,12 +1927,12 @@
         <v>74</v>
       </c>
       <c r="E94" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C95" t="s">
         <v>61</v>
@@ -1935,46 +1941,46 @@
         <v>74</v>
       </c>
       <c r="E95" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>112</v>
+      </c>
+      <c r="C96" t="s">
+        <v>61</v>
+      </c>
+      <c r="D96" t="s">
+        <v>74</v>
+      </c>
+      <c r="E96" t="s">
         <v>116</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>49</v>
-      </c>
-      <c r="B98" t="s">
-        <v>50</v>
-      </c>
-      <c r="C98" t="s">
-        <v>59</v>
-      </c>
-      <c r="D98" t="s">
-        <v>51</v>
-      </c>
-      <c r="E98" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
+        <v>49</v>
+      </c>
+      <c r="B99" t="s">
+        <v>50</v>
+      </c>
+      <c r="C99" t="s">
+        <v>59</v>
+      </c>
+      <c r="D99" t="s">
+        <v>51</v>
+      </c>
+      <c r="E99" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
         <v>25</v>
       </c>
-      <c r="B99" t="s">
+      <c r="B100" t="s">
         <v>118</v>
-      </c>
-      <c r="C99" t="s">
-        <v>60</v>
-      </c>
-      <c r="D99" t="s">
-        <v>57</v>
-      </c>
-      <c r="E99" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B100" t="s">
-        <v>119</v>
       </c>
       <c r="C100" t="s">
         <v>60</v>
@@ -1983,12 +1989,12 @@
         <v>57</v>
       </c>
       <c r="E100" t="s">
-        <v>93</v>
+        <v>121</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B101" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C101" t="s">
         <v>60</v>
@@ -1997,46 +2003,46 @@
         <v>57</v>
       </c>
       <c r="E101" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B102" t="s">
+        <v>120</v>
+      </c>
+      <c r="C102" t="s">
+        <v>60</v>
+      </c>
+      <c r="D102" t="s">
+        <v>57</v>
+      </c>
+      <c r="E102" t="s">
         <v>122</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>49</v>
-      </c>
-      <c r="B104" t="s">
-        <v>50</v>
-      </c>
-      <c r="C104" t="s">
-        <v>59</v>
-      </c>
-      <c r="D104" t="s">
-        <v>51</v>
-      </c>
-      <c r="E104" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
+        <v>49</v>
+      </c>
+      <c r="B105" t="s">
+        <v>50</v>
+      </c>
+      <c r="C105" t="s">
+        <v>59</v>
+      </c>
+      <c r="D105" t="s">
+        <v>51</v>
+      </c>
+      <c r="E105" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
         <v>5</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B106" t="s">
         <v>118</v>
-      </c>
-      <c r="C105" t="s">
-        <v>60</v>
-      </c>
-      <c r="D105" t="s">
-        <v>57</v>
-      </c>
-      <c r="E105" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B106" t="s">
-        <v>120</v>
       </c>
       <c r="C106" t="s">
         <v>60</v>
@@ -2045,46 +2051,46 @@
         <v>57</v>
       </c>
       <c r="E106" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
+        <v>120</v>
+      </c>
+      <c r="C107" t="s">
+        <v>60</v>
+      </c>
+      <c r="D107" t="s">
+        <v>57</v>
+      </c>
+      <c r="E107" t="s">
         <v>122</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>49</v>
-      </c>
-      <c r="B109" t="s">
-        <v>50</v>
-      </c>
-      <c r="C109" t="s">
-        <v>59</v>
-      </c>
-      <c r="D109" t="s">
-        <v>51</v>
-      </c>
-      <c r="E109" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
+        <v>49</v>
+      </c>
+      <c r="B110" t="s">
+        <v>50</v>
+      </c>
+      <c r="C110" t="s">
+        <v>59</v>
+      </c>
+      <c r="D110" t="s">
+        <v>51</v>
+      </c>
+      <c r="E110" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
         <v>30</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B111" t="s">
         <v>118</v>
-      </c>
-      <c r="C110" t="s">
-        <v>60</v>
-      </c>
-      <c r="D110" t="s">
-        <v>57</v>
-      </c>
-      <c r="E110" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B111" t="s">
-        <v>117</v>
       </c>
       <c r="C111" t="s">
         <v>60</v>
@@ -2093,34 +2099,48 @@
         <v>57</v>
       </c>
       <c r="E111" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C112" t="s">
         <v>60</v>
       </c>
       <c r="D112" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E112" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="113" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C113" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D113" t="s">
         <v>58</v>
       </c>
       <c r="E113" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="114" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
+        <v>124</v>
+      </c>
+      <c r="C114" t="s">
+        <v>61</v>
+      </c>
+      <c r="D114" t="s">
+        <v>58</v>
+      </c>
+      <c r="E114" t="s">
         <v>126</v>
       </c>
     </row>

</xml_diff>